<commit_message>
Change G coordinate in xls file Add rear piston and cylinder Group all parts into subsystems Change code to separate rear from front
</commit_message>
<xml_diff>
--- a/kinematics/geometries/VMS_front_rear.xlsx
+++ b/kinematics/geometries/VMS_front_rear.xlsx
@@ -193,9 +193,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>485280</xdr:colOff>
+      <xdr:colOff>484920</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>52920</xdr:rowOff>
+      <xdr:rowOff>52560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -209,7 +209,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2346840" y="146520"/>
-          <a:ext cx="3806280" cy="4668840"/>
+          <a:ext cx="3801960" cy="4668480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -235,9 +235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>218520</xdr:colOff>
+      <xdr:colOff>218160</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>35640</xdr:rowOff>
+      <xdr:rowOff>35280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -250,8 +250,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2619720" y="199800"/>
-          <a:ext cx="4370400" cy="5360040"/>
+          <a:off x="2619000" y="199800"/>
+          <a:ext cx="4365720" cy="5359680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -274,7 +274,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -388,13 +388,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>577.101</v>
+        <v>585.95</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>281.596</v>
+        <v>287.25</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1520.126</v>
+        <v>1520.13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -529,7 +529,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -643,13 +643,13 @@
         <v>10</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>606.198</v>
+        <v>616.11</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>158.313</v>
+        <v>153.79</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>-10.26</v>
+        <v>-8.21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>